<commit_message>
Added transactions and its handling
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Resource</t>
   </si>
@@ -39,12 +39,6 @@
     <t>/accounts/{id}</t>
   </si>
   <si>
-    <t>/client</t>
-  </si>
-  <si>
-    <t>/client/{id}</t>
-  </si>
-  <si>
     <t>Returns a list of accounts</t>
   </si>
   <si>
@@ -54,15 +48,9 @@
     <t>Create a new account</t>
   </si>
   <si>
-    <t>Not allowed</t>
-  </si>
-  <si>
     <t>Bulk update of accounts</t>
   </si>
   <si>
-    <t>Delete all accounts</t>
-  </si>
-  <si>
     <t>Returns a list of clients</t>
   </si>
   <si>
@@ -81,13 +69,43 @@
     <t>Update a specific account</t>
   </si>
   <si>
-    <t>Delete a specific account</t>
-  </si>
-  <si>
-    <t>Delete a specific client</t>
-  </si>
-  <si>
-    <t>Delete all client</t>
+    <t>Returns the last transfers (30 days period)</t>
+  </si>
+  <si>
+    <t>Create a new transfer</t>
+  </si>
+  <si>
+    <t>Returns a specific transfer</t>
+  </si>
+  <si>
+    <t>Returns transfers from a specific date</t>
+  </si>
+  <si>
+    <t>Returns transfers from a specific account</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Note: As all these data are sensible, the DELETE operations are not allowed. Instead of that, we can add a DEACTIVATED status. This is out of scope at this moment. Some POST operation are not allowed because doesn't make sense changes at this kind of system for that information after creation.</t>
+  </si>
+  <si>
+    <t>/transactions/transfers/{date}</t>
+  </si>
+  <si>
+    <t>/transactions/transfers</t>
+  </si>
+  <si>
+    <t>/transactions/transfers/{id}</t>
+  </si>
+  <si>
+    <t>/transactions/transfers/{fromAccount}</t>
+  </si>
+  <si>
+    <t>/clients</t>
+  </si>
+  <si>
+    <t>/clients/{id}</t>
   </si>
 </sst>
 </file>
@@ -130,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -140,6 +158,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,19 +463,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="13.19921875" customWidth="1"/>
-    <col min="2" max="2" width="20.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.296875" customWidth="1"/>
-    <col min="4" max="4" width="22.09765625" customWidth="1"/>
-    <col min="5" max="5" width="25.796875" customWidth="1"/>
+    <col min="1" max="1" width="27.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1">
@@ -479,16 +500,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -496,53 +517,154 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:E14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
TestResources have been added
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -90,22 +90,22 @@
     <t>Note: As all these data are sensible, the DELETE operations are not allowed. Instead of that, we can add a DEACTIVATED status. This is out of scope at this moment. Some POST operation are not allowed because doesn't make sense changes at this kind of system for that information after creation.</t>
   </si>
   <si>
-    <t>/transactions/transfers/{date}</t>
-  </si>
-  <si>
     <t>/transactions/transfers</t>
   </si>
   <si>
     <t>/transactions/transfers/{id}</t>
   </si>
   <si>
-    <t>/transactions/transfers/{fromAccount}</t>
-  </si>
-  <si>
     <t>/clients</t>
   </si>
   <si>
     <t>/clients/{id}</t>
+  </si>
+  <si>
+    <t>/transactions/transfers/from/{date}</t>
+  </si>
+  <si>
+    <t>/transactions/transfers/account/{fromAccount}</t>
   </si>
 </sst>
 </file>
@@ -466,12 +466,12 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="27.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.8984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.8984375" bestFit="1" customWidth="1"/>
@@ -531,7 +531,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>

</xml_diff>